<commit_message>
updated stencil Torc Map
</commit_message>
<xml_diff>
--- a/tempos/Livro1.xlsx
+++ b/tempos/Livro1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pinto\Desktop\faculdade\Mestrado\tese\tempos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B13346-33EC-4535-B535-6936E5827A31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D6510FE-C2FD-4EFC-BD04-0872B9BBC6C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{8EBD9DCE-4E05-454A-9645-960691A486AE}"/>
+    <workbookView xWindow="40920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8EBD9DCE-4E05-454A-9645-960691A486AE}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -35,8 +35,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="10">
   <si>
     <t>THREADS</t>
   </si>
@@ -63,6 +85,9 @@
   </si>
   <si>
     <t>% FASTER TORC_MAP</t>
+  </si>
+  <si>
+    <t>STENCIL</t>
   </si>
 </sst>
 </file>
@@ -106,7 +131,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -114,14 +139,33 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
-    <dxf>
-      <font>
-        <b/>
+  <dxfs count="42">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -129,6 +173,19 @@
     <dxf>
       <font>
         <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -136,6 +193,19 @@
     <dxf>
       <font>
         <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -143,6 +213,76 @@
     <dxf>
       <font>
         <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -150,6 +290,19 @@
     <dxf>
       <font>
         <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -157,31 +310,311 @@
     <dxf>
       <font>
         <b/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -235,17 +668,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4017355C-ACE8-404D-A030-86E9D188E3E9}" name="Tabela3" displayName="Tabela3" ref="C8:H18" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4017355C-ACE8-404D-A030-86E9D188E3E9}" name="Tabela3" displayName="Tabela3" ref="C8:H19" totalsRowCount="1" headerRowDxfId="41" dataDxfId="40">
   <autoFilter ref="C8:H18" xr:uid="{4017355C-ACE8-404D-A030-86E9D188E3E9}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{C98AF479-E221-4A14-B9BE-E7053BAA2634}" name="THREADS" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{208B8228-56D3-4A48-9160-A2535670BD90}" name="NO_TORCPY" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{61F68BFC-B467-47E2-A2C8-0E2199B59AB1}" name="WITH_TORCPY_MAP" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{595497DF-D8FC-4682-B02C-B2415D8B2188}" name="WITH_TORCPY_MINE" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{501D5899-B2F9-4108-B1C4-A071ECD87B58}" name="% FASTER NO_TORCPY" dataDxfId="3">
+    <tableColumn id="1" xr3:uid="{C98AF479-E221-4A14-B9BE-E7053BAA2634}" name="THREADS" dataDxfId="39" totalsRowDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{208B8228-56D3-4A48-9160-A2535670BD90}" name="NO_TORCPY" dataDxfId="38" totalsRowDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{61F68BFC-B467-47E2-A2C8-0E2199B59AB1}" name="WITH_TORCPY_MAP" dataDxfId="37" totalsRowDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{595497DF-D8FC-4682-B02C-B2415D8B2188}" name="WITH_TORCPY_MINE" dataDxfId="36" totalsRowDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{501D5899-B2F9-4108-B1C4-A071ECD87B58}" name="% FASTER NO_TORCPY" dataDxfId="35" totalsRowDxfId="7">
       <calculatedColumnFormula>100 - (D9*100/F9)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{57B518AE-7406-429F-9B76-C5A7CE4DDB54}" name="% FASTER TORC_MAP" dataDxfId="1">
+    <tableColumn id="6" xr3:uid="{57B518AE-7406-429F-9B76-C5A7CE4DDB54}" name="% FASTER TORC_MAP" dataDxfId="34" totalsRowDxfId="6">
       <calculatedColumnFormula>100 - (E9*100/F9)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -254,17 +687,17 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{267D8E00-0183-45B4-8B95-DB3E6BD88ACE}" name="Tabela33" displayName="Tabela33" ref="C23:H33" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{267D8E00-0183-45B4-8B95-DB3E6BD88ACE}" name="Tabela33" displayName="Tabela33" ref="C23:H34" totalsRowCount="1" headerRowDxfId="33" dataDxfId="32">
   <autoFilter ref="C23:H33" xr:uid="{267D8E00-0183-45B4-8B95-DB3E6BD88ACE}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{7BC9BE73-34AA-44B8-98E5-EB8775B1093D}" name="THREADS" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{3B191EA7-49F8-4C72-AA5C-C3D7BE96919E}" name="NO_TORCPY" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{4E00C22E-8E2F-4BD5-A368-74D302F963C0}" name="WITH_TORCPY_MAP" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{F7078830-C246-4828-A4CA-68768101B0FE}" name="WITH_TORCPY_MINE" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{D1DD9F50-83AC-421D-A7BD-E20E8D9A0611}" name="% FASTER NO_TORCPY" dataDxfId="2">
+    <tableColumn id="1" xr3:uid="{7BC9BE73-34AA-44B8-98E5-EB8775B1093D}" name="THREADS" dataDxfId="31" totalsRowDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{3B191EA7-49F8-4C72-AA5C-C3D7BE96919E}" name="NO_TORCPY" dataDxfId="30" totalsRowDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{4E00C22E-8E2F-4BD5-A368-74D302F963C0}" name="WITH_TORCPY_MAP" dataDxfId="29" totalsRowDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{F7078830-C246-4828-A4CA-68768101B0FE}" name="WITH_TORCPY_MINE" dataDxfId="28" totalsRowDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{D1DD9F50-83AC-421D-A7BD-E20E8D9A0611}" name="% FASTER NO_TORCPY" dataDxfId="27" totalsRowDxfId="1">
       <calculatedColumnFormula>100 - (D24*100/F24)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{D9E37E4F-7CDC-4FDC-9291-42693CAD1CD5}" name="% SLOWER TORC_MAP" dataDxfId="0">
+    <tableColumn id="6" xr3:uid="{D9E37E4F-7CDC-4FDC-9291-42693CAD1CD5}" name="% SLOWER TORC_MAP" dataDxfId="26" totalsRowDxfId="0">
       <calculatedColumnFormula>(E24*100/F24) - 100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -272,10 +705,31 @@
 </table>
 </file>
 
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3676447E-83EC-481B-BAB7-FC31903A21E7}" name="Tabela332" displayName="Tabela332" ref="C41:H52" totalsRowCount="1" headerRowDxfId="25" dataDxfId="24">
+  <autoFilter ref="C41:H51" xr:uid="{3676447E-83EC-481B-BAB7-FC31903A21E7}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{547AC1A3-2A11-4C9B-B162-7377C62A83AA}" name="THREADS" dataDxfId="23" totalsRowDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{829B1D67-909C-47B5-BDFB-6BCABB018C83}" name="NO_TORCPY" dataDxfId="22" totalsRowDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{77F01A88-0E90-4311-A77A-9CFB20F91830}" name="WITH_TORCPY_MAP" dataDxfId="21" totalsRowDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{907655F2-A1EC-4098-AD88-83A40E44C685}" name="WITH_TORCPY_MINE" dataDxfId="20" totalsRowDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{CD390048-0FDB-44C7-8D50-5BC3B37B5032}" name="% FASTER NO_TORCPY" totalsRowFunction="custom" dataDxfId="18" totalsRowDxfId="13">
+      <calculatedColumnFormula>100 - (D42*100/F42)</calculatedColumnFormula>
+      <totalsRowFormula array="1">SUM(Tabela332[% FASTER NO_TORCPY]/10)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{5588AC35-A2AA-4678-A606-34333CE63B29}" name="% SLOWER TORC_MAP" totalsRowFunction="custom" dataDxfId="19" totalsRowDxfId="12">
+      <calculatedColumnFormula>(E42*100/F42) - 100</calculatedColumnFormula>
+      <totalsRowFormula array="1">SUM(Tabela332[% SLOWER TORC_MAP]/10)</totalsRowFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema Office 2013 - 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -313,7 +767,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -419,7 +873,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -561,7 +1015,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -569,10 +1023,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EF78862-5946-4DF0-A9D6-D2FEDB594540}">
-  <dimension ref="C7:H33"/>
+  <dimension ref="C7:H52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="K49" sqref="K49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -829,6 +1283,14 @@
         <v>100</v>
       </c>
     </row>
+    <row r="19" spans="3:8" x14ac:dyDescent="0.45">
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+    </row>
     <row r="22" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C22" s="2" t="s">
         <v>4</v>
@@ -873,11 +1335,11 @@
         <v>16.815936803817699</v>
       </c>
       <c r="G24" s="1">
-        <f t="shared" ref="G24:H33" si="2">100 - (D24*100/F24)</f>
+        <f>100 - (D24*100/F24)</f>
         <v>7.5527308493800973</v>
       </c>
       <c r="H24" s="1">
-        <f t="shared" ref="H24:H33" si="3">(E24*100/F24) - 100</f>
+        <f t="shared" ref="H24:H33" si="2">(E24*100/F24) - 100</f>
         <v>165.11702467467245</v>
       </c>
     </row>
@@ -895,11 +1357,11 @@
         <v>40.839495420455897</v>
       </c>
       <c r="G25" s="1">
+        <f t="shared" ref="G24:G33" si="3">100 - (D25*100/F25)</f>
+        <v>7.1487232314262741</v>
+      </c>
+      <c r="H25" s="1">
         <f t="shared" si="2"/>
-        <v>7.1487232314262741</v>
-      </c>
-      <c r="H25" s="1">
-        <f t="shared" si="3"/>
         <v>46.199104075660188</v>
       </c>
     </row>
@@ -917,11 +1379,11 @@
         <v>22.404618740081698</v>
       </c>
       <c r="G26" s="1">
+        <f t="shared" si="3"/>
+        <v>5.6288524995725737</v>
+      </c>
+      <c r="H26" s="1">
         <f t="shared" si="2"/>
-        <v>5.6288524995725737</v>
-      </c>
-      <c r="H26" s="1">
-        <f t="shared" si="3"/>
         <v>174.25827361664909</v>
       </c>
     </row>
@@ -939,11 +1401,11 @@
         <v>66.797793865203801</v>
       </c>
       <c r="G27" s="1">
+        <f t="shared" si="3"/>
+        <v>3.6723634479769203</v>
+      </c>
+      <c r="H27" s="1">
         <f t="shared" si="2"/>
-        <v>3.6723634479769203</v>
-      </c>
-      <c r="H27" s="1">
-        <f t="shared" si="3"/>
         <v>59.201087778575442</v>
       </c>
     </row>
@@ -961,11 +1423,11 @@
         <v>35.932974576950002</v>
       </c>
       <c r="G28" s="1">
+        <f t="shared" si="3"/>
+        <v>2.3177549498628025</v>
+      </c>
+      <c r="H28" s="1">
         <f t="shared" si="2"/>
-        <v>2.3177549498628025</v>
-      </c>
-      <c r="H28" s="1">
-        <f t="shared" si="3"/>
         <v>210.49295818056379</v>
       </c>
     </row>
@@ -983,11 +1445,11 @@
         <v>66.517926216125403</v>
       </c>
       <c r="G29" s="1">
+        <f t="shared" si="3"/>
+        <v>10.59398493179134</v>
+      </c>
+      <c r="H29" s="1">
         <f t="shared" si="2"/>
-        <v>10.59398493179134</v>
-      </c>
-      <c r="H29" s="1">
-        <f t="shared" si="3"/>
         <v>220.47887040149715</v>
       </c>
     </row>
@@ -1005,11 +1467,11 @@
         <v>131.02463364601101</v>
       </c>
       <c r="G30" s="1">
+        <f t="shared" si="3"/>
+        <v>11.527736392181737</v>
+      </c>
+      <c r="H30" s="1">
         <f t="shared" si="2"/>
-        <v>11.527736392181737</v>
-      </c>
-      <c r="H30" s="1">
-        <f t="shared" si="3"/>
         <v>222.10943904659865</v>
       </c>
     </row>
@@ -1021,11 +1483,11 @@
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
       <c r="G31" s="1" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H31" s="1" t="e">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H31" s="1" t="e">
-        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1037,11 +1499,11 @@
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
       <c r="G32" s="1" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H32" s="1" t="e">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H32" s="1" t="e">
-        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1053,24 +1515,304 @@
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H33" s="1" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H33" s="1" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+    </row>
+    <row r="34" spans="3:8" x14ac:dyDescent="0.45">
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
+    </row>
+    <row r="37" spans="3:8" x14ac:dyDescent="0.45">
+      <c r="E37" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
+    </row>
+    <row r="40" spans="3:8" x14ac:dyDescent="0.45">
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+    </row>
+    <row r="41" spans="3:8" x14ac:dyDescent="0.45">
+      <c r="C41" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="3:8" x14ac:dyDescent="0.45">
+      <c r="C42" s="1">
+        <v>96</v>
+      </c>
+      <c r="D42" s="1">
+        <v>28.813753366470301</v>
+      </c>
+      <c r="E42" s="1">
+        <v>28.725849866867001</v>
+      </c>
+      <c r="F42" s="1">
+        <v>27.853418588638299</v>
+      </c>
+      <c r="G42" s="1">
+        <f t="shared" ref="G42:G51" si="4">100 - (D42*100/F42)</f>
+        <v>-3.4478165571522794</v>
+      </c>
+      <c r="H42" s="1">
+        <f t="shared" ref="H42:H51" si="5">(E42*100/F42) - 100</f>
+        <v>3.1322233407448863</v>
+      </c>
+    </row>
+    <row r="43" spans="3:8" x14ac:dyDescent="0.45">
+      <c r="C43" s="1">
+        <v>65</v>
+      </c>
+      <c r="D43" s="1">
+        <v>39.340156555175703</v>
+      </c>
+      <c r="E43" s="1">
+        <v>39.820995092391897</v>
+      </c>
+      <c r="F43" s="1">
+        <v>39.104621648788402</v>
+      </c>
+      <c r="G43" s="1">
+        <f t="shared" si="4"/>
+        <v>-0.6023198702770145</v>
+      </c>
+      <c r="H43" s="1">
+        <f t="shared" si="5"/>
+        <v>1.8319406080372858</v>
+      </c>
+    </row>
+    <row r="44" spans="3:8" x14ac:dyDescent="0.45">
+      <c r="C44" s="1">
+        <v>64</v>
+      </c>
+      <c r="D44" s="1">
+        <v>40.397493600845301</v>
+      </c>
+      <c r="E44" s="1">
+        <v>38.4539184570312</v>
+      </c>
+      <c r="F44" s="1">
+        <v>40.724493026733398</v>
+      </c>
+      <c r="G44" s="1">
+        <f t="shared" si="4"/>
+        <v>0.80295517902074209</v>
+      </c>
+      <c r="H44" s="1">
+        <f t="shared" si="5"/>
+        <v>-5.5754520214940158</v>
+      </c>
+    </row>
+    <row r="45" spans="3:8" x14ac:dyDescent="0.45">
+      <c r="C45" s="1">
+        <v>33</v>
+      </c>
+      <c r="D45" s="1">
+        <v>76.809633731841998</v>
+      </c>
+      <c r="E45" s="1">
+        <v>72.981305837631197</v>
+      </c>
+      <c r="F45" s="1">
+        <v>72.495656490325899</v>
+      </c>
+      <c r="G45" s="1">
+        <f t="shared" si="4"/>
+        <v>-5.9506699440562585</v>
+      </c>
+      <c r="H45" s="1">
+        <f t="shared" si="5"/>
+        <v>0.66990130280440496</v>
+      </c>
+    </row>
+    <row r="46" spans="3:8" x14ac:dyDescent="0.45">
+      <c r="C46" s="1">
+        <v>32</v>
+      </c>
+      <c r="D46" s="1">
+        <v>79.858301877975407</v>
+      </c>
+      <c r="E46" s="1">
+        <v>71.353382587432804</v>
+      </c>
+      <c r="F46" s="1">
+        <v>74.347388744354205</v>
+      </c>
+      <c r="G46" s="1">
+        <f t="shared" si="4"/>
+        <v>-7.4123829050279681</v>
+      </c>
+      <c r="H46" s="1">
+        <f t="shared" si="5"/>
+        <v>-4.0270495137581577</v>
+      </c>
+    </row>
+    <row r="47" spans="3:8" x14ac:dyDescent="0.45">
+      <c r="C47" s="1">
+        <v>16</v>
+      </c>
+      <c r="D47" s="1">
+        <v>86.824947595596299</v>
+      </c>
+      <c r="E47" s="1">
+        <v>81.003350257873507</v>
+      </c>
+      <c r="F47" s="1">
+        <v>79.841888427734304</v>
+      </c>
+      <c r="G47" s="1">
+        <f t="shared" si="4"/>
+        <v>-8.7461097243240005</v>
+      </c>
+      <c r="H47" s="1">
+        <f t="shared" si="5"/>
+        <v>1.4547023536278942</v>
+      </c>
+    </row>
+    <row r="48" spans="3:8" x14ac:dyDescent="0.45">
+      <c r="C48" s="1">
+        <v>8</v>
+      </c>
+      <c r="D48" s="1">
+        <v>150.98461818695</v>
+      </c>
+      <c r="E48" s="1">
+        <v>151.43423056602401</v>
+      </c>
+      <c r="F48" s="1">
+        <v>154.462168931961</v>
+      </c>
+      <c r="G48" s="1">
+        <f t="shared" si="4"/>
+        <v>2.2513931851771645</v>
+      </c>
+      <c r="H48" s="1">
+        <f t="shared" si="5"/>
+        <v>-1.9603106617457655</v>
+      </c>
+    </row>
+    <row r="49" spans="3:8" x14ac:dyDescent="0.45">
+      <c r="C49" s="1">
+        <v>4</v>
+      </c>
+      <c r="D49" s="1">
+        <v>304.69980812072703</v>
+      </c>
+      <c r="E49" s="1">
+        <v>296.98543405532803</v>
+      </c>
+      <c r="F49" s="1">
+        <v>294.11314558982798</v>
+      </c>
+      <c r="G49" s="1">
+        <f t="shared" si="4"/>
+        <v>-3.5995203511451592</v>
+      </c>
+      <c r="H49" s="1">
+        <f t="shared" si="5"/>
+        <v>0.97659302502097489</v>
+      </c>
+    </row>
+    <row r="50" spans="3:8" x14ac:dyDescent="0.45">
+      <c r="C50" s="1">
+        <v>2</v>
+      </c>
+      <c r="D50" s="1">
+        <v>574.90111565589905</v>
+      </c>
+      <c r="E50" s="1">
+        <v>561.32839250564496</v>
+      </c>
+      <c r="F50" s="1">
+        <v>606.58675003051701</v>
+      </c>
+      <c r="G50" s="1">
+        <f t="shared" si="4"/>
+        <v>5.2235948729549193</v>
+      </c>
+      <c r="H50" s="1">
+        <f t="shared" si="5"/>
+        <v>-7.461151685656688</v>
+      </c>
+    </row>
+    <row r="51" spans="3:8" x14ac:dyDescent="0.45">
+      <c r="C51" s="1">
+        <v>1</v>
+      </c>
+      <c r="D51" s="1">
+        <v>1147.3579795360499</v>
+      </c>
+      <c r="E51" s="1">
+        <v>1158.19151115417</v>
+      </c>
+      <c r="F51" s="1">
+        <v>1147.2181239128099</v>
+      </c>
+      <c r="G51" s="1">
+        <f t="shared" si="4"/>
+        <v>-1.2190848481637317E-2</v>
+      </c>
+      <c r="H51" s="1">
+        <f t="shared" si="5"/>
+        <v>0.95652143325048655</v>
+      </c>
+    </row>
+    <row r="52" spans="3:8" x14ac:dyDescent="0.45">
+      <c r="C52" s="1"/>
+      <c r="D52" s="1"/>
+      <c r="E52" s="1"/>
+      <c r="F52" s="4"/>
+      <c r="G52" s="4" cm="1">
+        <f t="array" ref="G52">SUM(Tabela332[% FASTER NO_TORCPY]/10)</f>
+        <v>-2.1493066963311493</v>
+      </c>
+      <c r="H52" s="4" cm="1">
+        <f t="array" ref="H52">SUM(Tabela332[% SLOWER TORC_MAP]/10)</f>
+        <v>-1.0002081819168696</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="C22:H22"/>
     <mergeCell ref="C7:H7"/>
+    <mergeCell ref="C40:H40"/>
+    <mergeCell ref="E37:G37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="2">
+  <tableParts count="3">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated times of stencil
</commit_message>
<xml_diff>
--- a/tempos/Livro1.xlsx
+++ b/tempos/Livro1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pinto\Desktop\faculdade\Mestrado\tese\tempos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D6510FE-C2FD-4EFC-BD04-0872B9BBC6C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98754D8B-D18D-4DA5-9B6B-E1BB75078008}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8EBD9DCE-4E05-454A-9645-960691A486AE}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{8EBD9DCE-4E05-454A-9645-960691A486AE}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="11">
   <si>
     <t>THREADS</t>
   </si>
@@ -89,12 +89,15 @@
   <si>
     <t>STENCIL</t>
   </si>
+  <si>
+    <t>AVERAGE</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,16 +113,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -127,11 +150,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -142,7 +189,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -167,7 +229,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -187,7 +248,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -207,7 +267,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -270,6 +329,13 @@
     <dxf>
       <font>
         <b/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -290,6 +356,13 @@
     <dxf>
       <font>
         <b/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -310,6 +383,13 @@
     <dxf>
       <font>
         <b/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -330,6 +410,13 @@
     <dxf>
       <font>
         <b/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -349,6 +436,12 @@
     <dxf>
       <font>
         <b/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -368,6 +461,12 @@
     <dxf>
       <font>
         <b/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -387,6 +486,56 @@
     <dxf>
       <font>
         <b/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -407,6 +556,13 @@
     <dxf>
       <font>
         <b/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -427,6 +583,13 @@
     <dxf>
       <font>
         <b/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -447,6 +610,13 @@
     <dxf>
       <font>
         <b/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -466,6 +636,12 @@
     <dxf>
       <font>
         <b/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -485,6 +661,12 @@
     <dxf>
       <font>
         <b/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -499,129 +681,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -671,14 +730,14 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4017355C-ACE8-404D-A030-86E9D188E3E9}" name="Tabela3" displayName="Tabela3" ref="C8:H19" totalsRowCount="1" headerRowDxfId="41" dataDxfId="40">
   <autoFilter ref="C8:H18" xr:uid="{4017355C-ACE8-404D-A030-86E9D188E3E9}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{C98AF479-E221-4A14-B9BE-E7053BAA2634}" name="THREADS" dataDxfId="39" totalsRowDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{208B8228-56D3-4A48-9160-A2535670BD90}" name="NO_TORCPY" dataDxfId="38" totalsRowDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{61F68BFC-B467-47E2-A2C8-0E2199B59AB1}" name="WITH_TORCPY_MAP" dataDxfId="37" totalsRowDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{595497DF-D8FC-4682-B02C-B2415D8B2188}" name="WITH_TORCPY_MINE" dataDxfId="36" totalsRowDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{501D5899-B2F9-4108-B1C4-A071ECD87B58}" name="% FASTER NO_TORCPY" dataDxfId="35" totalsRowDxfId="7">
+    <tableColumn id="1" xr3:uid="{C98AF479-E221-4A14-B9BE-E7053BAA2634}" name="THREADS" dataDxfId="18" totalsRowDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{208B8228-56D3-4A48-9160-A2535670BD90}" name="NO_TORCPY" dataDxfId="16" totalsRowDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{61F68BFC-B467-47E2-A2C8-0E2199B59AB1}" name="WITH_TORCPY_MAP" dataDxfId="14" totalsRowDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{595497DF-D8FC-4682-B02C-B2415D8B2188}" name="WITH_TORCPY_MINE" dataDxfId="12" totalsRowDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{501D5899-B2F9-4108-B1C4-A071ECD87B58}" name="% FASTER NO_TORCPY" dataDxfId="10" totalsRowDxfId="9">
       <calculatedColumnFormula>100 - (D9*100/F9)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{57B518AE-7406-429F-9B76-C5A7CE4DDB54}" name="% FASTER TORC_MAP" dataDxfId="34" totalsRowDxfId="6">
+    <tableColumn id="6" xr3:uid="{57B518AE-7406-429F-9B76-C5A7CE4DDB54}" name="% FASTER TORC_MAP" dataDxfId="8" totalsRowDxfId="7">
       <calculatedColumnFormula>100 - (E9*100/F9)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -687,17 +746,17 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{267D8E00-0183-45B4-8B95-DB3E6BD88ACE}" name="Tabela33" displayName="Tabela33" ref="C23:H34" totalsRowCount="1" headerRowDxfId="33" dataDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{267D8E00-0183-45B4-8B95-DB3E6BD88ACE}" name="Tabela33" displayName="Tabela33" ref="C23:H34" totalsRowCount="1" headerRowDxfId="39" dataDxfId="38">
   <autoFilter ref="C23:H33" xr:uid="{267D8E00-0183-45B4-8B95-DB3E6BD88ACE}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{7BC9BE73-34AA-44B8-98E5-EB8775B1093D}" name="THREADS" dataDxfId="31" totalsRowDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{3B191EA7-49F8-4C72-AA5C-C3D7BE96919E}" name="NO_TORCPY" dataDxfId="30" totalsRowDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{4E00C22E-8E2F-4BD5-A368-74D302F963C0}" name="WITH_TORCPY_MAP" dataDxfId="29" totalsRowDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{F7078830-C246-4828-A4CA-68768101B0FE}" name="WITH_TORCPY_MINE" dataDxfId="28" totalsRowDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{D1DD9F50-83AC-421D-A7BD-E20E8D9A0611}" name="% FASTER NO_TORCPY" dataDxfId="27" totalsRowDxfId="1">
+    <tableColumn id="1" xr3:uid="{7BC9BE73-34AA-44B8-98E5-EB8775B1093D}" name="THREADS" dataDxfId="37" totalsRowDxfId="36"/>
+    <tableColumn id="2" xr3:uid="{3B191EA7-49F8-4C72-AA5C-C3D7BE96919E}" name="NO_TORCPY" dataDxfId="35" totalsRowDxfId="34"/>
+    <tableColumn id="3" xr3:uid="{4E00C22E-8E2F-4BD5-A368-74D302F963C0}" name="WITH_TORCPY_MAP" dataDxfId="33" totalsRowDxfId="32"/>
+    <tableColumn id="4" xr3:uid="{F7078830-C246-4828-A4CA-68768101B0FE}" name="WITH_TORCPY_MINE" dataDxfId="31" totalsRowDxfId="30"/>
+    <tableColumn id="5" xr3:uid="{D1DD9F50-83AC-421D-A7BD-E20E8D9A0611}" name="% FASTER NO_TORCPY" dataDxfId="29" totalsRowDxfId="28">
       <calculatedColumnFormula>100 - (D24*100/F24)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{D9E37E4F-7CDC-4FDC-9291-42693CAD1CD5}" name="% SLOWER TORC_MAP" dataDxfId="26" totalsRowDxfId="0">
+    <tableColumn id="6" xr3:uid="{D9E37E4F-7CDC-4FDC-9291-42693CAD1CD5}" name="% SLOWER TORC_MAP" dataDxfId="27" totalsRowDxfId="26">
       <calculatedColumnFormula>(E24*100/F24) - 100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -709,17 +768,17 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3676447E-83EC-481B-BAB7-FC31903A21E7}" name="Tabela332" displayName="Tabela332" ref="C41:H52" totalsRowCount="1" headerRowDxfId="25" dataDxfId="24">
   <autoFilter ref="C41:H51" xr:uid="{3676447E-83EC-481B-BAB7-FC31903A21E7}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{547AC1A3-2A11-4C9B-B162-7377C62A83AA}" name="THREADS" dataDxfId="23" totalsRowDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{829B1D67-909C-47B5-BDFB-6BCABB018C83}" name="NO_TORCPY" dataDxfId="22" totalsRowDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{77F01A88-0E90-4311-A77A-9CFB20F91830}" name="WITH_TORCPY_MAP" dataDxfId="21" totalsRowDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{907655F2-A1EC-4098-AD88-83A40E44C685}" name="WITH_TORCPY_MINE" dataDxfId="20" totalsRowDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{CD390048-0FDB-44C7-8D50-5BC3B37B5032}" name="% FASTER NO_TORCPY" totalsRowFunction="custom" dataDxfId="18" totalsRowDxfId="13">
+    <tableColumn id="1" xr3:uid="{547AC1A3-2A11-4C9B-B162-7377C62A83AA}" name="THREADS" dataDxfId="23" totalsRowDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{829B1D67-909C-47B5-BDFB-6BCABB018C83}" name="NO_TORCPY" dataDxfId="22" totalsRowDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{77F01A88-0E90-4311-A77A-9CFB20F91830}" name="WITH_TORCPY_MAP" dataDxfId="21" totalsRowDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{907655F2-A1EC-4098-AD88-83A40E44C685}" name="WITH_TORCPY_MINE" dataDxfId="20" totalsRowDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{CD390048-0FDB-44C7-8D50-5BC3B37B5032}" name="% FASTER NO_TORCPY" totalsRowFunction="custom" dataDxfId="19" totalsRowDxfId="1">
       <calculatedColumnFormula>100 - (D42*100/F42)</calculatedColumnFormula>
       <totalsRowFormula array="1">SUM(Tabela332[% FASTER NO_TORCPY]/10)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{5588AC35-A2AA-4678-A606-34333CE63B29}" name="% SLOWER TORC_MAP" totalsRowFunction="custom" dataDxfId="19" totalsRowDxfId="12">
-      <calculatedColumnFormula>(E42*100/F42) - 100</calculatedColumnFormula>
-      <totalsRowFormula array="1">SUM(Tabela332[% SLOWER TORC_MAP]/10)</totalsRowFormula>
+    <tableColumn id="6" xr3:uid="{5588AC35-A2AA-4678-A606-34333CE63B29}" name="% FASTER TORC_MAP" totalsRowFunction="custom" dataDxfId="6" totalsRowDxfId="0">
+      <calculatedColumnFormula>100 - (E42*100/F42)</calculatedColumnFormula>
+      <totalsRowFormula array="1">SUM(Tabela332[% FASTER TORC_MAP]/10)</totalsRowFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1023,10 +1082,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EF78862-5946-4DF0-A9D6-D2FEDB594540}">
-  <dimension ref="C7:H52"/>
+  <dimension ref="A7:H105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="K49" sqref="K49"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="F101" sqref="F101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1287,9 +1346,9 @@
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
     </row>
     <row r="22" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C22" s="2" t="s">
@@ -1357,7 +1416,7 @@
         <v>40.839495420455897</v>
       </c>
       <c r="G25" s="1">
-        <f t="shared" ref="G24:G33" si="3">100 - (D25*100/F25)</f>
+        <f t="shared" ref="G25:G33" si="3">100 - (D25*100/F25)</f>
         <v>7.1487232314262741</v>
       </c>
       <c r="H25" s="1">
@@ -1527,9 +1586,9 @@
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
-      <c r="H34" s="4"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
     </row>
     <row r="37" spans="3:8" x14ac:dyDescent="0.45">
       <c r="E37" s="3" t="s">
@@ -1563,7 +1622,7 @@
         <v>2</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="42" spans="3:8" x14ac:dyDescent="0.45">
@@ -1571,21 +1630,21 @@
         <v>96</v>
       </c>
       <c r="D42" s="1">
-        <v>28.813753366470301</v>
+        <v>28.18661539</v>
       </c>
       <c r="E42" s="1">
-        <v>28.725849866867001</v>
+        <v>28.562558970000001</v>
       </c>
       <c r="F42" s="1">
-        <v>27.853418588638299</v>
+        <v>28.066862579999999</v>
       </c>
       <c r="G42" s="1">
         <f t="shared" ref="G42:G51" si="4">100 - (D42*100/F42)</f>
-        <v>-3.4478165571522794</v>
+        <v>-0.42666974143855896</v>
       </c>
       <c r="H42" s="1">
-        <f t="shared" ref="H42:H51" si="5">(E42*100/F42) - 100</f>
-        <v>3.1322233407448863</v>
+        <f t="shared" ref="H42:H51" si="5">100 - (E42*100/F42)</f>
+        <v>-1.7661268287009335</v>
       </c>
     </row>
     <row r="43" spans="3:8" x14ac:dyDescent="0.45">
@@ -1593,21 +1652,21 @@
         <v>65</v>
       </c>
       <c r="D43" s="1">
-        <v>39.340156555175703</v>
+        <v>39.188588299999999</v>
       </c>
       <c r="E43" s="1">
-        <v>39.820995092391897</v>
+        <v>38.717339199999998</v>
       </c>
       <c r="F43" s="1">
-        <v>39.104621648788402</v>
+        <v>38.803967710000002</v>
       </c>
       <c r="G43" s="1">
         <f t="shared" si="4"/>
-        <v>-0.6023198702770145</v>
+        <v>-0.99118882088153271</v>
       </c>
       <c r="H43" s="1">
         <f t="shared" si="5"/>
-        <v>1.8319406080372858</v>
+        <v>0.22324652635374775</v>
       </c>
     </row>
     <row r="44" spans="3:8" x14ac:dyDescent="0.45">
@@ -1615,21 +1674,21 @@
         <v>64</v>
       </c>
       <c r="D44" s="1">
-        <v>40.397493600845301</v>
+        <v>41.058056200000003</v>
       </c>
       <c r="E44" s="1">
-        <v>38.4539184570312</v>
+        <v>39.453190169999999</v>
       </c>
       <c r="F44" s="1">
-        <v>40.724493026733398</v>
+        <v>39.539218429999998</v>
       </c>
       <c r="G44" s="1">
         <f t="shared" si="4"/>
-        <v>0.80295517902074209</v>
+        <v>-3.8413449489117824</v>
       </c>
       <c r="H44" s="1">
         <f t="shared" si="5"/>
-        <v>-5.5754520214940158</v>
+        <v>0.21757703722015265</v>
       </c>
     </row>
     <row r="45" spans="3:8" x14ac:dyDescent="0.45">
@@ -1637,21 +1696,21 @@
         <v>33</v>
       </c>
       <c r="D45" s="1">
-        <v>76.809633731841998</v>
+        <v>75.058801729999999</v>
       </c>
       <c r="E45" s="1">
-        <v>72.981305837631197</v>
+        <v>71.73426517</v>
       </c>
       <c r="F45" s="1">
-        <v>72.495656490325899</v>
+        <v>75.059882720000004</v>
       </c>
       <c r="G45" s="1">
         <f t="shared" si="4"/>
-        <v>-5.9506699440562585</v>
+        <v>1.4401701159556524E-3</v>
       </c>
       <c r="H45" s="1">
         <f t="shared" si="5"/>
-        <v>0.66990130280440496</v>
+        <v>4.4306191663071672</v>
       </c>
     </row>
     <row r="46" spans="3:8" x14ac:dyDescent="0.45">
@@ -1659,21 +1718,21 @@
         <v>32</v>
       </c>
       <c r="D46" s="1">
-        <v>79.858301877975407</v>
+        <v>76.030074909999996</v>
       </c>
       <c r="E46" s="1">
-        <v>71.353382587432804</v>
+        <v>73.807288009999994</v>
       </c>
       <c r="F46" s="1">
-        <v>74.347388744354205</v>
+        <v>76.004185519999993</v>
       </c>
       <c r="G46" s="1">
         <f t="shared" si="4"/>
-        <v>-7.4123829050279681</v>
+        <v>-3.4063110896951798E-2</v>
       </c>
       <c r="H46" s="1">
         <f t="shared" si="5"/>
-        <v>-4.0270495137581577</v>
+        <v>2.8904954312310878</v>
       </c>
     </row>
     <row r="47" spans="3:8" x14ac:dyDescent="0.45">
@@ -1681,21 +1740,21 @@
         <v>16</v>
       </c>
       <c r="D47" s="1">
-        <v>86.824947595596299</v>
+        <v>82.231000899999998</v>
       </c>
       <c r="E47" s="1">
-        <v>81.003350257873507</v>
+        <v>78.91267053</v>
       </c>
       <c r="F47" s="1">
-        <v>79.841888427734304</v>
+        <v>80.914210879999999</v>
       </c>
       <c r="G47" s="1">
         <f t="shared" si="4"/>
-        <v>-8.7461097243240005</v>
+        <v>-1.6273903010101236</v>
       </c>
       <c r="H47" s="1">
         <f t="shared" si="5"/>
-        <v>1.4547023536278942</v>
+        <v>2.4736573813571425</v>
       </c>
     </row>
     <row r="48" spans="3:8" x14ac:dyDescent="0.45">
@@ -1703,21 +1762,21 @@
         <v>8</v>
       </c>
       <c r="D48" s="1">
-        <v>150.98461818695</v>
+        <v>153.12796499999999</v>
       </c>
       <c r="E48" s="1">
-        <v>151.43423056602401</v>
+        <v>151.19525300000001</v>
       </c>
       <c r="F48" s="1">
-        <v>154.462168931961</v>
+        <v>158.4099698</v>
       </c>
       <c r="G48" s="1">
         <f t="shared" si="4"/>
-        <v>2.2513931851771645</v>
+        <v>3.334389121258468</v>
       </c>
       <c r="H48" s="1">
         <f t="shared" si="5"/>
-        <v>-1.9603106617457655</v>
+        <v>4.5544587939186556</v>
       </c>
     </row>
     <row r="49" spans="3:8" x14ac:dyDescent="0.45">
@@ -1725,21 +1784,21 @@
         <v>4</v>
       </c>
       <c r="D49" s="1">
-        <v>304.69980812072703</v>
+        <v>301.03539050000001</v>
       </c>
       <c r="E49" s="1">
-        <v>296.98543405532803</v>
+        <v>293.4845335</v>
       </c>
       <c r="F49" s="1">
-        <v>294.11314558982798</v>
+        <v>300.80607930000002</v>
       </c>
       <c r="G49" s="1">
         <f t="shared" si="4"/>
-        <v>-3.5995203511451592</v>
+        <v>-7.6232235908790358E-2</v>
       </c>
       <c r="H49" s="1">
         <f t="shared" si="5"/>
-        <v>0.97659302502097489</v>
+        <v>2.4339753428646986</v>
       </c>
     </row>
     <row r="50" spans="3:8" x14ac:dyDescent="0.45">
@@ -1747,21 +1806,21 @@
         <v>2</v>
       </c>
       <c r="D50" s="1">
-        <v>574.90111565589905</v>
+        <v>584.45763620000002</v>
       </c>
       <c r="E50" s="1">
-        <v>561.32839250564496</v>
+        <v>581.23957289999998</v>
       </c>
       <c r="F50" s="1">
-        <v>606.58675003051701</v>
+        <v>623.20541530000003</v>
       </c>
       <c r="G50" s="1">
         <f t="shared" si="4"/>
-        <v>5.2235948729549193</v>
+        <v>6.2174971764883509</v>
       </c>
       <c r="H50" s="1">
         <f t="shared" si="5"/>
-        <v>-7.461151685656688</v>
+        <v>6.7338699840723422</v>
       </c>
     </row>
     <row r="51" spans="3:8" x14ac:dyDescent="0.45">
@@ -1769,35 +1828,602 @@
         <v>1</v>
       </c>
       <c r="D51" s="1">
-        <v>1147.3579795360499</v>
+        <v>1136.5505029999999</v>
       </c>
       <c r="E51" s="1">
-        <v>1158.19151115417</v>
+        <v>1152.1473309999999</v>
       </c>
       <c r="F51" s="1">
-        <v>1147.2181239128099</v>
+        <v>1175.8128730000001</v>
       </c>
       <c r="G51" s="1">
         <f t="shared" si="4"/>
-        <v>-1.2190848481637317E-2</v>
+        <v>3.3391682385501724</v>
       </c>
       <c r="H51" s="1">
         <f t="shared" si="5"/>
-        <v>0.95652143325048655</v>
+        <v>2.0126962838584461</v>
       </c>
     </row>
     <row r="52" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
-      <c r="F52" s="4"/>
-      <c r="G52" s="4" cm="1">
+      <c r="F52" s="1"/>
+      <c r="G52" s="1" cm="1">
         <f t="array" ref="G52">SUM(Tabela332[% FASTER NO_TORCPY]/10)</f>
-        <v>-2.1493066963311493</v>
-      </c>
-      <c r="H52" s="4" cm="1">
-        <f t="array" ref="H52">SUM(Tabela332[% SLOWER TORC_MAP]/10)</f>
-        <v>-1.0002081819168696</v>
+        <v>0.58956055473652103</v>
+      </c>
+      <c r="H52" s="1" cm="1">
+        <f t="array" ref="H52">SUM(Tabela332[% FASTER TORC_MAP]/10)</f>
+        <v>2.4204469118482508</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A70" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B70" t="s">
+        <v>10</v>
+      </c>
+      <c r="C70" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A71" s="4">
+        <v>96</v>
+      </c>
+      <c r="B71">
+        <f>(C71+D71+E71)/3</f>
+        <v>28.186615387598636</v>
+      </c>
+      <c r="C71" s="7">
+        <v>28.813753366470301</v>
+      </c>
+      <c r="D71">
+        <v>27.403955698013299</v>
+      </c>
+      <c r="E71">
+        <v>28.3421370983123</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A72" s="5">
+        <v>65</v>
+      </c>
+      <c r="B72">
+        <f t="shared" ref="B72:B80" si="6">(C72+D72+E72)/3</f>
+        <v>39.188588301340673</v>
+      </c>
+      <c r="C72" s="8">
+        <v>39.340156555175703</v>
+      </c>
+      <c r="D72">
+        <v>38.195333719253497</v>
+      </c>
+      <c r="E72">
+        <v>40.030274629592803</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A73" s="4">
+        <v>64</v>
+      </c>
+      <c r="B73">
+        <f t="shared" si="6"/>
+        <v>41.058056195576938</v>
+      </c>
+      <c r="C73" s="7">
+        <v>40.397493600845301</v>
+      </c>
+      <c r="D73">
+        <v>42.326999187469397</v>
+      </c>
+      <c r="E73">
+        <v>40.449675798416102</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A74" s="5">
+        <v>33</v>
+      </c>
+      <c r="B74">
+        <f t="shared" si="6"/>
+        <v>75.058801730473803</v>
+      </c>
+      <c r="C74" s="8">
+        <v>76.809633731841998</v>
+      </c>
+      <c r="D74">
+        <v>71.258037567138601</v>
+      </c>
+      <c r="E74">
+        <v>77.108733892440796</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A75" s="4">
+        <v>32</v>
+      </c>
+      <c r="B75">
+        <f t="shared" si="6"/>
+        <v>76.030074914296435</v>
+      </c>
+      <c r="C75" s="7">
+        <v>79.858301877975407</v>
+      </c>
+      <c r="D75">
+        <v>74.466809272766099</v>
+      </c>
+      <c r="E75">
+        <v>73.765113592147799</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A76" s="5">
+        <v>16</v>
+      </c>
+      <c r="B76">
+        <f t="shared" si="6"/>
+        <v>82.231000900268498</v>
+      </c>
+      <c r="C76" s="8">
+        <v>86.824947595596299</v>
+      </c>
+      <c r="D76">
+        <v>82.930469274520803</v>
+      </c>
+      <c r="E76">
+        <v>76.937585830688406</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A77" s="4">
+        <v>8</v>
+      </c>
+      <c r="B77">
+        <f t="shared" si="6"/>
+        <v>153.127964973449</v>
+      </c>
+      <c r="C77" s="7">
+        <v>150.98461818695</v>
+      </c>
+      <c r="D77">
+        <v>149.437199831008</v>
+      </c>
+      <c r="E77">
+        <v>158.96207690238899</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A78" s="5">
+        <v>4</v>
+      </c>
+      <c r="B78">
+        <f t="shared" si="6"/>
+        <v>301.03539053598973</v>
+      </c>
+      <c r="C78" s="8">
+        <v>304.69980812072703</v>
+      </c>
+      <c r="D78">
+        <v>299.93067431449799</v>
+      </c>
+      <c r="E78">
+        <v>298.47568917274401</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A79" s="4">
+        <v>2</v>
+      </c>
+      <c r="B79">
+        <f t="shared" si="6"/>
+        <v>584.45763619740762</v>
+      </c>
+      <c r="C79" s="7">
+        <v>574.90111565589905</v>
+      </c>
+      <c r="D79">
+        <v>592.40464091300896</v>
+      </c>
+      <c r="E79">
+        <v>586.06715202331497</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A80" s="5">
+        <v>1</v>
+      </c>
+      <c r="B80">
+        <f t="shared" si="6"/>
+        <v>1136.5505027770932</v>
+      </c>
+      <c r="C80" s="8">
+        <v>1147.3579795360499</v>
+      </c>
+      <c r="D80">
+        <v>1134.93759751319</v>
+      </c>
+      <c r="E80">
+        <v>1127.35593128204</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A82" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C82" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A83" s="4">
+        <v>96</v>
+      </c>
+      <c r="B83">
+        <f>(C83+D83+E83)/3</f>
+        <v>28.562558968861833</v>
+      </c>
+      <c r="C83" s="7">
+        <v>28.725849866867001</v>
+      </c>
+      <c r="D83">
+        <v>28.781089782714801</v>
+      </c>
+      <c r="E83">
+        <v>28.180737257003699</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A84" s="5">
+        <v>65</v>
+      </c>
+      <c r="B84">
+        <f t="shared" ref="B84:B92" si="7">(C84+D84+E84)/3</f>
+        <v>38.71733919779453</v>
+      </c>
+      <c r="C84" s="8">
+        <v>39.820995092391897</v>
+      </c>
+      <c r="D84">
+        <v>38.4277245998382</v>
+      </c>
+      <c r="E84">
+        <v>37.903297901153501</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A85" s="4">
+        <v>64</v>
+      </c>
+      <c r="B85">
+        <f t="shared" si="7"/>
+        <v>39.4531901677449</v>
+      </c>
+      <c r="C85" s="7">
+        <v>38.4539184570312</v>
+      </c>
+      <c r="D85">
+        <v>38.885028123855498</v>
+      </c>
+      <c r="E85">
+        <v>41.020623922348001</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A86" s="5">
+        <v>33</v>
+      </c>
+      <c r="B86">
+        <f t="shared" si="7"/>
+        <v>71.734265168507861</v>
+      </c>
+      <c r="C86" s="8">
+        <v>72.981305837631197</v>
+      </c>
+      <c r="D86">
+        <v>72.338082313537598</v>
+      </c>
+      <c r="E86">
+        <v>69.883407354354802</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A87" s="4">
+        <v>32</v>
+      </c>
+      <c r="B87">
+        <f t="shared" si="7"/>
+        <v>73.807288010915059</v>
+      </c>
+      <c r="C87" s="7">
+        <v>71.353382587432804</v>
+      </c>
+      <c r="D87">
+        <v>75.526950597763005</v>
+      </c>
+      <c r="E87">
+        <v>74.541530847549396</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A88" s="5">
+        <v>16</v>
+      </c>
+      <c r="B88">
+        <f t="shared" si="7"/>
+        <v>78.912670532862293</v>
+      </c>
+      <c r="C88" s="8">
+        <v>81.003350257873507</v>
+      </c>
+      <c r="D88">
+        <v>78.382187128067002</v>
+      </c>
+      <c r="E88">
+        <v>77.352474212646399</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A89" s="4">
+        <v>8</v>
+      </c>
+      <c r="B89">
+        <f t="shared" si="7"/>
+        <v>151.19525297482767</v>
+      </c>
+      <c r="C89" s="7">
+        <v>151.43423056602401</v>
+      </c>
+      <c r="D89">
+        <v>150.38002038002</v>
+      </c>
+      <c r="E89">
+        <v>151.77150797843899</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A90" s="5">
+        <v>4</v>
+      </c>
+      <c r="B90">
+        <f t="shared" si="7"/>
+        <v>293.4845335483547</v>
+      </c>
+      <c r="C90" s="8">
+        <v>296.98543405532803</v>
+      </c>
+      <c r="D90">
+        <v>289.26285648345902</v>
+      </c>
+      <c r="E90">
+        <v>294.20531010627701</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A91" s="4">
+        <v>2</v>
+      </c>
+      <c r="B91">
+        <f t="shared" si="7"/>
+        <v>581.23957292238799</v>
+      </c>
+      <c r="C91" s="7">
+        <v>561.32839250564496</v>
+      </c>
+      <c r="D91">
+        <v>587.06899070739701</v>
+      </c>
+      <c r="E91">
+        <v>595.32133555412202</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A92" s="5">
+        <v>1</v>
+      </c>
+      <c r="B92">
+        <f t="shared" si="7"/>
+        <v>1152.1473308404231</v>
+      </c>
+      <c r="C92" s="8">
+        <v>1158.19151115417</v>
+      </c>
+      <c r="D92">
+        <v>1159.5043864250099</v>
+      </c>
+      <c r="E92">
+        <v>1138.7460949420899</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A95" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C95" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A96" s="4">
+        <v>96</v>
+      </c>
+      <c r="B96">
+        <f>(C96+D96+E96)/3</f>
+        <v>28.066862583160361</v>
+      </c>
+      <c r="C96" s="7">
+        <v>27.853418588638299</v>
+      </c>
+      <c r="D96">
+        <v>27.916335344314501</v>
+      </c>
+      <c r="E96">
+        <v>28.430833816528299</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A97" s="5">
+        <v>65</v>
+      </c>
+      <c r="B97">
+        <f t="shared" ref="B97:B105" si="8">(C97+D97+E97)/3</f>
+        <v>38.803967714309664</v>
+      </c>
+      <c r="C97" s="8">
+        <v>39.104621648788402</v>
+      </c>
+      <c r="D97">
+        <v>38.741544008254998</v>
+      </c>
+      <c r="E97">
+        <v>38.565737485885599</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A98" s="4">
+        <v>64</v>
+      </c>
+      <c r="B98">
+        <f t="shared" si="8"/>
+        <v>39.539218425750704</v>
+      </c>
+      <c r="C98" s="7">
+        <v>40.724493026733398</v>
+      </c>
+      <c r="D98">
+        <v>38.294193983078003</v>
+      </c>
+      <c r="E98">
+        <v>39.598968267440704</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A99" s="5">
+        <v>33</v>
+      </c>
+      <c r="B99">
+        <f t="shared" si="8"/>
+        <v>75.059882720311421</v>
+      </c>
+      <c r="C99" s="8">
+        <v>72.495656490325899</v>
+      </c>
+      <c r="D99">
+        <v>75.548486232757497</v>
+      </c>
+      <c r="E99">
+        <v>77.135505437850895</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A100" s="4">
+        <v>32</v>
+      </c>
+      <c r="B100">
+        <f t="shared" si="8"/>
+        <v>76.004185517628926</v>
+      </c>
+      <c r="C100" s="7">
+        <v>74.347388744354205</v>
+      </c>
+      <c r="D100">
+        <v>76.276735067367497</v>
+      </c>
+      <c r="E100">
+        <v>77.388432741165104</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A101" s="5">
+        <v>16</v>
+      </c>
+      <c r="B101">
+        <f t="shared" si="8"/>
+        <v>80.914210875828999</v>
+      </c>
+      <c r="C101" s="8">
+        <v>79.841888427734304</v>
+      </c>
+      <c r="D101">
+        <v>84.209939479827796</v>
+      </c>
+      <c r="E101">
+        <v>78.690804719924898</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A102" s="4">
+        <v>8</v>
+      </c>
+      <c r="B102">
+        <f t="shared" si="8"/>
+        <v>158.409969806671</v>
+      </c>
+      <c r="C102" s="7">
+        <v>154.462168931961</v>
+      </c>
+      <c r="D102">
+        <v>162.78553104400601</v>
+      </c>
+      <c r="E102">
+        <v>157.98220944404599</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A103" s="5">
+        <v>4</v>
+      </c>
+      <c r="B103">
+        <f t="shared" si="8"/>
+        <v>300.80607930819133</v>
+      </c>
+      <c r="C103" s="8">
+        <v>294.11314558982798</v>
+      </c>
+      <c r="D103">
+        <v>292.09741353988602</v>
+      </c>
+      <c r="E103">
+        <v>316.20767879485999</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A104" s="4">
+        <v>2</v>
+      </c>
+      <c r="B104">
+        <f t="shared" si="8"/>
+        <v>623.20541532834329</v>
+      </c>
+      <c r="C104" s="7">
+        <v>606.58675003051701</v>
+      </c>
+      <c r="D104">
+        <v>631.86411261558499</v>
+      </c>
+      <c r="E104">
+        <v>631.165383338928</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A105" s="5">
+        <v>1</v>
+      </c>
+      <c r="B105">
+        <f t="shared" si="8"/>
+        <v>1175.8128729661269</v>
+      </c>
+      <c r="C105" s="8">
+        <v>1147.2181239128099</v>
+      </c>
+      <c r="D105">
+        <v>1206.6539056301101</v>
+      </c>
+      <c r="E105">
+        <v>1173.5665893554601</v>
       </c>
     </row>
   </sheetData>

</xml_diff>